<commit_message>
add registering user with data provided form excel
</commit_message>
<xml_diff>
--- a/src/test/resources/logInData.xlsx
+++ b/src/test/resources/logInData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProgramowanie\Nauka\seleniumtests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A9D0F96-6110-4F00-B0B9-E08FA5ECF97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65413528-F908-4EB2-9A75-A16736DCCB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="3384" windowWidth="17280" windowHeight="8976" xr2:uid="{600F0D02-A97E-4F9D-8EA6-BC9AD2E301D2}"/>
+    <workbookView xWindow="2400" yWindow="1116" windowWidth="17280" windowHeight="8976" xr2:uid="{600F0D02-A97E-4F9D-8EA6-BC9AD2E301D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -44,32 +44,41 @@
     <t>password</t>
   </si>
   <si>
-    <t>tst111@test.com</t>
-  </si>
-  <si>
     <t>SecurePassw1!</t>
   </si>
   <si>
-    <t>tst222@test.com</t>
-  </si>
-  <si>
     <t>SecurePassw2!</t>
   </si>
   <si>
-    <t>tst333@test.com</t>
-  </si>
-  <si>
     <t>SecurePassw3!</t>
+  </si>
+  <si>
+    <t>tst11@test.com</t>
+  </si>
+  <si>
+    <t>tst22@test.com</t>
+  </si>
+  <si>
+    <t>tst33@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -93,13 +102,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,7 +447,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,30 +461,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FE1FF116-F91E-425B-BB2B-D8F28E6CF97E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{CA242FB1-D0D7-4C86-A25B-880056719C36}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{137C2B70-38C2-4309-AFAD-9AC5DE3A51A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add reports to RegisterTest
</commit_message>
<xml_diff>
--- a/src/test/resources/logInData.xlsx
+++ b/src/test/resources/logInData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProgramowanie\Nauka\seleniumtests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65413528-F908-4EB2-9A75-A16736DCCB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03EE048-6F51-4FD7-A8C6-51087EC944FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="1116" windowWidth="17280" windowHeight="8976" xr2:uid="{600F0D02-A97E-4F9D-8EA6-BC9AD2E301D2}"/>
   </bookViews>
@@ -53,13 +53,13 @@
     <t>SecurePassw3!</t>
   </si>
   <si>
-    <t>tst11@test.com</t>
-  </si>
-  <si>
-    <t>tst22@test.com</t>
-  </si>
-  <si>
-    <t>tst33@test.com</t>
+    <t>tst11d@test.com</t>
+  </si>
+  <si>
+    <t>tst22d@test.com</t>
+  </si>
+  <si>
+    <t>tst33d@test.com</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,8 +487,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{FE1FF116-F91E-425B-BB2B-D8F28E6CF97E}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{CA242FB1-D0D7-4C86-A25B-880056719C36}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{137C2B70-38C2-4309-AFAD-9AC5DE3A51A0}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{137C2B70-38C2-4309-AFAD-9AC5DE3A51A0}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{CA242FB1-D0D7-4C86-A25B-880056719C36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>